<commit_message>
updated subs productIds for Fortune INTL
</commit_message>
<xml_diff>
--- a/assets/Sub-IAP_ProductIDs.xlsx
+++ b/assets/Sub-IAP_ProductIDs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="1600" windowWidth="23400" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="18280" windowHeight="14020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Title</t>
   </si>
@@ -271,13 +271,31 @@
   </si>
   <si>
     <t>6 Month Product ID</t>
+  </si>
+  <si>
+    <t>com.international.fortune.ipad.inapp.subs.3</t>
+  </si>
+  <si>
+    <t>com.international.fortune.ipad.inapp.subs.9</t>
+  </si>
+  <si>
+    <t>com.tahk.fortune.ipad.inapp.subs.3</t>
+  </si>
+  <si>
+    <t>com.tahk.fortune.ipad.inapp.subs.9</t>
+  </si>
+  <si>
+    <t>com.emea.fortune.ipad.inapp.subs.3</t>
+  </si>
+  <si>
+    <t>com.emea.fortune.ipad.inapp.subs.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -316,6 +334,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -350,13 +373,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -786,13 +810,13 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="42.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="43.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="4"/>
@@ -879,27 +903,39 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">

</xml_diff>